<commit_message>
add course-assistant && small fix on investment-decision-analysis
</commit_message>
<xml_diff>
--- a/tasks/finalpool/course-assistant/initial_workspace/nlp_statistics.xlsx
+++ b/tasks/finalpool/course-assistant/initial_workspace/nlp_statistics.xlsx
@@ -404,64 +404,64 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>学号</v>
+        <v>Student ID</v>
       </c>
       <c r="B1" t="str">
-        <v>姓名</v>
+        <v>Name</v>
       </c>
       <c r="C1" t="str">
-        <v>作业1</v>
+        <v>Assignment1</v>
       </c>
       <c r="D1" t="str">
-        <v>作业2</v>
+        <v>Assignment2</v>
       </c>
       <c r="E1" t="str">
-        <v>作业3</v>
+        <v>Assignment3</v>
       </c>
       <c r="F1" t="str">
-        <v>作业4</v>
+        <v>Assignment4</v>
       </c>
       <c r="G1" t="str">
-        <v>作业5</v>
+        <v>Assignment5</v>
       </c>
       <c r="H1" t="str">
-        <v>作业6</v>
+        <v>Assignment6</v>
       </c>
       <c r="I1" t="str">
-        <v>作业7</v>
+        <v>Assignment7</v>
       </c>
       <c r="J1" t="str">
-        <v>作业8</v>
+        <v>Assignment8</v>
       </c>
       <c r="K1" t="str">
-        <v>作业9</v>
+        <v>Assignment9</v>
       </c>
       <c r="L1" t="str">
-        <v>作业10</v>
+        <v>Assignment10</v>
       </c>
       <c r="M1" t="str">
-        <v>作业11</v>
+        <v>Assignment11</v>
       </c>
       <c r="N1" t="str">
-        <v>小作业</v>
+        <v>Quiz1</v>
       </c>
       <c r="O1" t="str">
-        <v>大作业</v>
+        <v>Project1</v>
       </c>
       <c r="P1" t="str">
-        <v>汇报作业</v>
+        <v>Pre</v>
       </c>
       <c r="Q1" t="str">
-        <v>作业平均</v>
+        <v>Averaged Score</v>
       </c>
       <c r="R1" t="str">
         <v/>
       </c>
       <c r="S1" t="str">
-        <v>备注_x000d_</v>
+        <v>Note</v>
       </c>
       <c r="T1" t="str">
-        <v>联系信息</v>
+        <v>Email</v>
       </c>
     </row>
     <row r="2">
@@ -469,7 +469,7 @@
         <v>1800016633</v>
       </c>
       <c r="B2" t="str">
-        <v>李珂</v>
+        <v>John Reed</v>
       </c>
       <c r="C2" t="str">
         <v>10</v>
@@ -523,7 +523,7 @@
         <v>_x000d_</v>
       </c>
       <c r="T2" t="str">
-        <v>like2@cse.ust.hk_x000d_</v>
+        <v>john_reed@mcp.com</v>
       </c>
     </row>
     <row r="3">
@@ -531,7 +531,7 @@
         <v>1800090104</v>
       </c>
       <c r="B3" t="str">
-        <v>留美琪</v>
+        <v>Andrew Diaz</v>
       </c>
       <c r="C3" t="str">
         <v>10</v>
@@ -585,7 +585,7 @@
         <v>_x000d_</v>
       </c>
       <c r="T3" t="str">
-        <v>meiqi06@cse.ust.hk_x000d_</v>
+        <v>diaza48@mcp.com</v>
       </c>
     </row>
     <row r="4">
@@ -593,7 +593,7 @@
         <v>1800093002</v>
       </c>
       <c r="B4" t="str">
-        <v>林丽琪</v>
+        <v>Matthew Bailey</v>
       </c>
       <c r="C4" t="str">
         <v>9</v>
@@ -647,7 +647,7 @@
         <v>_x000d_</v>
       </c>
       <c r="T4" t="str">
-        <v>liqi@cse.ust.hk_x000d_</v>
+        <v>matthew.bailey32@mcp.com</v>
       </c>
     </row>
     <row r="5">
@@ -655,7 +655,7 @@
         <v>1900016620</v>
       </c>
       <c r="B5" t="str">
-        <v>丁楠</v>
+        <v>Ryan Gomez</v>
       </c>
       <c r="C5" t="str">
         <v>10</v>
@@ -709,7 +709,7 @@
         <v>_x000d_</v>
       </c>
       <c r="T5" t="str">
-        <v>dingnan01@cse.ust.hk_x000d_</v>
+        <v>ryang13@mcp.com</v>
       </c>
     </row>
     <row r="6">
@@ -717,7 +717,7 @@
         <v>1900016628</v>
       </c>
       <c r="B6" t="str">
-        <v>陈淑芬</v>
+        <v>Patricia Watson</v>
       </c>
       <c r="C6" t="str">
         <v>10</v>
@@ -771,7 +771,7 @@
         <v>_x000d_</v>
       </c>
       <c r="T6" t="str">
-        <v>cjb06@cse.ust.hk_x000d_</v>
+        <v>pwatson23@mcp.com</v>
       </c>
     </row>
     <row r="7">
@@ -779,7 +779,7 @@
         <v>2000012117</v>
       </c>
       <c r="B7" t="str">
-        <v>陈劲柏</v>
+        <v>Kimberly Murphy</v>
       </c>
       <c r="C7" t="str">
         <v>10</v>
@@ -833,7 +833,7 @@
         <v>_x000d_</v>
       </c>
       <c r="T7" t="str">
-        <v>cjb08@cse.ust.hk_x000d_</v>
+        <v>kimberly.murphy@mcp.com</v>
       </c>
     </row>
     <row r="8">
@@ -841,7 +841,7 @@
         <v>2000012969</v>
       </c>
       <c r="B8" t="str">
-        <v>郑一杭</v>
+        <v>Edward Ruiz</v>
       </c>
       <c r="C8" t="str">
         <v>10</v>
@@ -895,7 +895,7 @@
         <v>_x000d_</v>
       </c>
       <c r="T8" t="str">
-        <v>yihang02@cse.ust.hk_x000d_</v>
+        <v>edward.ruiz@mcp.com</v>
       </c>
     </row>
     <row r="9">
@@ -903,7 +903,7 @@
         <v>2000014178</v>
       </c>
       <c r="B9" t="str">
-        <v>姜子涵</v>
+        <v>Shirley Edwards</v>
       </c>
       <c r="C9" t="str">
         <v>10</v>
@@ -957,7 +957,7 @@
         <v>_x000d_</v>
       </c>
       <c r="T9" t="str">
-        <v>zihan10@cse.ust.hk_x000d_</v>
+        <v>shirley_edwards@mcp.com</v>
       </c>
     </row>
     <row r="10">
@@ -965,7 +965,7 @@
         <v>2000014180</v>
       </c>
       <c r="B10" t="str">
-        <v>陈佳豪</v>
+        <v>Catherine Murphy</v>
       </c>
       <c r="C10" t="str">
         <v>10</v>
@@ -1019,7 +1019,7 @@
         <v>_x000d_</v>
       </c>
       <c r="T10" t="str">
-        <v>cjh03@cse.ust.hk_x000d_</v>
+        <v>murphyc@mcp.com</v>
       </c>
     </row>
     <row r="11">
@@ -1027,7 +1027,7 @@
         <v>2000014200</v>
       </c>
       <c r="B11" t="str">
-        <v>黄依灵</v>
+        <v>Sandra Miller</v>
       </c>
       <c r="C11" t="str">
         <v>9.5</v>
@@ -1078,10 +1078,10 @@
         <v/>
       </c>
       <c r="S11" t="str">
-        <v>已退课_x000d_</v>
+        <v>Already withdrew from the course</v>
       </c>
       <c r="T11" t="str">
-        <v>kewincpt93@gmail.com_x000d_</v>
+        <v>sandra.miller@mcp.com</v>
       </c>
     </row>
     <row r="12">
@@ -1089,7 +1089,7 @@
         <v>2000016605</v>
       </c>
       <c r="B12" t="str">
-        <v>齐浩博</v>
+        <v>Carol Carter</v>
       </c>
       <c r="C12" t="str">
         <v>9.5</v>
@@ -1143,7 +1143,7 @@
         <v>_x000d_</v>
       </c>
       <c r="T12" t="str">
-        <v>haobo09@cse.ust.hk_x000d_</v>
+        <v>carterc23@mcp.com</v>
       </c>
     </row>
     <row r="13">
@@ -1151,7 +1151,7 @@
         <v>2000016606</v>
       </c>
       <c r="B13" t="str">
-        <v>赵晖</v>
+        <v>Michelle Brooks</v>
       </c>
       <c r="C13" t="str">
         <v>10</v>
@@ -1205,7 +1205,7 @@
         <v>_x000d_</v>
       </c>
       <c r="T13" t="str">
-        <v>zh2000@cse.ust.hk_x000d_</v>
+        <v>michelle_brooks26@mcp.com</v>
       </c>
     </row>
     <row r="14">
@@ -1213,7 +1213,7 @@
         <v>2000016613</v>
       </c>
       <c r="B14" t="str">
-        <v>朱晓钟</v>
+        <v>Steven Morgan</v>
       </c>
       <c r="C14" t="str">
         <v>9.5</v>
@@ -1267,7 +1267,7 @@
         <v>_x000d_</v>
       </c>
       <c r="T14" t="str">
-        <v>bennettb47@mcp.com</v>
+        <v>smorgan@mcp.com</v>
       </c>
     </row>
     <row r="15">
@@ -1275,7 +1275,7 @@
         <v>2000016630</v>
       </c>
       <c r="B15" t="str">
-        <v>韦杨珂</v>
+        <v>Carolyn Alvarez</v>
       </c>
       <c r="C15" t="str">
         <v>9.5</v>
@@ -1329,7 +1329,7 @@
         <v/>
       </c>
       <c r="T15" t="str">
-        <v>gortiz78@mcp.com</v>
+        <v>calvarez@mcp.com</v>
       </c>
     </row>
     <row r="16">
@@ -1337,7 +1337,7 @@
         <v>2100016613</v>
       </c>
       <c r="B16" t="str">
-        <v>朱丽丽</v>
+        <v>Jennifer Castillo</v>
       </c>
       <c r="C16" t="str">
         <v>9.5</v>
@@ -1382,7 +1382,7 @@
         <v>98</v>
       </c>
       <c r="T16" t="str">
-        <v>mcpllm.bench@gmail.com</v>
+        <v>castilloj@mcp.com</v>
       </c>
     </row>
     <row r="17">
@@ -1390,13 +1390,13 @@
         <v>106666</v>
       </c>
       <c r="B17" t="str">
-        <v>lekun</v>
+        <v>Andrew Moore</v>
       </c>
       <c r="S17" t="str">
-        <v>旁听教师账户</v>
+        <v>Auditing teacher</v>
       </c>
       <c r="T17" t="str">
-        <v>mcpllm.bench@gmail.com</v>
+        <v>moorea@mcp.com</v>
       </c>
     </row>
   </sheetData>

</xml_diff>